<commit_message>
Solved zipping issue, fixed index page
</commit_message>
<xml_diff>
--- a/source/DSO comparison.xlsx
+++ b/source/DSO comparison.xlsx
@@ -8,13 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jibrilsharafi/Personal/EnergyMe-Home/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1DA7D7F-336C-5147-A3C4-113ADE06A279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C8E707-47AC-5142-BA9F-E04255100E66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{F09C8B9D-A9D0-9640-90EA-F6C802E5DACE}"/>
   </bookViews>
   <sheets>
     <sheet name="Scalea" sheetId="2" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Scalea!$A$2:$A$8</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Scalea!$K$1</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Scalea!$A$2:$A$8</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Scalea!$K$1</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Scalea!$K$2:$K$8</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Scalea!$L$1</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Scalea!$L$2:$L$8</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Scalea!$K$2:$K$8</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Scalea!$L$1</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Scalea!$L$2:$L$8</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Scalea!$A$2:$A$8</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Scalea!$K$1</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Scalea!$K$2:$K$8</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Scalea!$L$1</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Scalea!$L$2:$L$8</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -79,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Timestamp</t>
   </si>
@@ -111,7 +128,10 @@
     <t>Relative difference [kWh]</t>
   </si>
   <si>
-    <t>Total</t>
+    <t>Total DSO [kWh]</t>
+  </si>
+  <si>
+    <t>Total EnergyMe [kWh]</t>
   </si>
 </sst>
 </file>
@@ -123,7 +143,7 @@
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -150,6 +170,17 @@
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Google Sans Text"/>
     </font>
   </fonts>
   <fills count="2">
@@ -178,25 +209,37 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="12">
     <dxf>
       <numFmt numFmtId="165" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -223,28 +266,2237 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Total</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> consumption</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Scalea!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total DSO [kWh]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Scalea!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy\ h:mm</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>45884.568055555559</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45884.867361111108</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45885.563888888886</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45885.840277777781</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45886.49722222222</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45886.902777777781</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45887.631944444445</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Scalea!$I$2:$I$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-33B6-8C48-B763-2DEF8C787A72}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Scalea!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total EnergyMe [kWh]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Scalea!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy\ h:mm</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>45884.568055555559</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45884.867361111108</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45885.563888888886</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45885.840277777781</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45886.49722222222</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45886.902777777781</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45887.631944444445</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Scalea!$J$2:$J$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.9430000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.0489999999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.582000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17.470700000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22.460299999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30.058999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-33B6-8C48-B763-2DEF8C787A72}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1211091040"/>
+        <c:axId val="1210581296"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1211091040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="m/d/yy\ h:mm" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1210581296"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1210581296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1211091040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Difference</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> DSO vs EnergyMe</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Scalea!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Absolute difference [kWh]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Scalea!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy\ h:mm</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>45884.568055555559</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45884.867361111108</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45885.563888888886</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45885.840277777781</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45886.49722222222</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45886.902777777781</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45887.631944444445</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Scalea!$K$2:$K$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-5.699999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.95100000000000051</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.58200000000000074</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.52929999999999922</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.5397000000000034</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.8999999999997499E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-32AB-AC46-B89E-88859C27493C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Scalea!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Relative difference [kWh]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Scalea!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy\ h:mm</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>45884.568055555559</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45884.867361111108</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45885.563888888886</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45885.840277777781</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45886.49722222222</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45886.902777777781</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45887.631944444445</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Scalea!$L$2:$L$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1.8999999999999979E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-9.5100000000000046E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.2909090909090975E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-2.9405555555555511E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-2.3465217391304496E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.9666666666665832E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-32AB-AC46-B89E-88859C27493C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1211091040"/>
+        <c:axId val="1210581296"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1211091040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="m/d/yy\ h:mm" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1210581296"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1210581296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1211091040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>297180</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>5080</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACCAB686-0359-D1B9-F78B-96DFDBC644D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1366520</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04EAB17F-5517-0D48-9B26-105BF97EB699}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4C15CE87-9103-3543-9609-61C6C7FA6FB0}" name="Table2" displayName="Table2" ref="A1:J7" totalsRowCount="1">
-  <autoFilter ref="A1:J6" xr:uid="{4C15CE87-9103-3543-9609-61C6C7FA6FB0}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{A85D948A-57A5-5F43-A54C-ACFC33A5E4FB}" name="Timestamp" totalsRowLabel="Total" dataDxfId="7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4C15CE87-9103-3543-9609-61C6C7FA6FB0}" name="Table2" displayName="Table2" ref="A1:L8">
+  <autoFilter ref="A1:L8" xr:uid="{4C15CE87-9103-3543-9609-61C6C7FA6FB0}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{A85D948A-57A5-5F43-A54C-ACFC33A5E4FB}" name="Timestamp" totalsRowLabel="Total" dataDxfId="11"/>
     <tableColumn id="2" xr3:uid="{D6F6B36F-5FCE-A84C-978A-9C1F96ED9634}" name="F1 [kWh]"/>
     <tableColumn id="3" xr3:uid="{EA87CE77-AEED-0C47-8F0A-47E93AF456DB}" name="F2 [kWh]"/>
     <tableColumn id="4" xr3:uid="{3A46886D-4E24-C649-8490-584ADD26F4D2}" name="F3  [kWh]"/>
     <tableColumn id="5" xr3:uid="{20D5B3D8-8D91-2C46-B385-F7AE272CE7F0}" name="Total [kWh]">
       <calculatedColumnFormula>SUM(Table2[[#This Row],[F1 '[kWh']]:[F3  '[kWh']]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{8A786C7A-843E-584F-B63E-AB2662379C23}" name="EnergyMe [kWh]" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{0A5C6413-28B4-4543-8978-2FCF4D3326FE}" name="Increment DSO [kWh]" totalsRowFunction="sum" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{FF11CD81-381A-C243-8371-22A55DAC9E15}" name="Increment EnergyMe [kWh]" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="1">
+    <tableColumn id="6" xr3:uid="{8A786C7A-843E-584F-B63E-AB2662379C23}" name="EnergyMe [kWh]" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{0A5C6413-28B4-4543-8978-2FCF4D3326FE}" name="Increment DSO [kWh]" totalsRowFunction="sum" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{FF11CD81-381A-C243-8371-22A55DAC9E15}" name="Increment EnergyMe [kWh]" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="7">
       <calculatedColumnFormula>F2-F1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{73F09D0E-1573-0B46-8186-9C024A8A8ADB}" name="Absolute difference [kWh]" totalsRowFunction="custom" dataDxfId="3">
-      <calculatedColumnFormula>Table2[[#This Row],[Increment EnergyMe '[kWh']]]-Table2[[#This Row],[Increment DSO '[kWh']]]</calculatedColumnFormula>
+    <tableColumn id="11" xr3:uid="{3FA9DF38-E45D-524A-82F0-951557DF5CC3}" name="Total DSO [kWh]" dataDxfId="6" totalsRowDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{E217CBC8-E899-9C42-B17F-7883D9374421}" name="Total EnergyMe [kWh]" dataDxfId="4" totalsRowDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{73F09D0E-1573-0B46-8186-9C024A8A8ADB}" name="Absolute difference [kWh]" totalsRowFunction="custom" dataDxfId="2">
+      <calculatedColumnFormula>Table2[[#This Row],[Total EnergyMe '[kWh']]]-Table2[[#This Row],[Total DSO '[kWh']]]</calculatedColumnFormula>
       <totalsRowFormula>Table2[[#Totals],[Increment EnergyMe '[kWh']]]-Table2[[#Totals],[Increment DSO '[kWh']]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{B13FC2DE-827C-8342-B2A2-6D3CEABA3857}" name="Relative difference [kWh]" totalsRowFunction="custom" dataDxfId="2" totalsRowDxfId="0">
-      <calculatedColumnFormula>Table2[[#This Row],[Absolute difference '[kWh']]]/Table2[[#This Row],[Increment DSO '[kWh']]]</calculatedColumnFormula>
+    <tableColumn id="10" xr3:uid="{B13FC2DE-827C-8342-B2A2-6D3CEABA3857}" name="Relative difference [kWh]" totalsRowFunction="custom" dataDxfId="1" totalsRowDxfId="0">
+      <calculatedColumnFormula>Table2[[#This Row],[Absolute difference '[kWh']]]/Table2[[#This Row],[Total DSO '[kWh']]]</calculatedColumnFormula>
       <totalsRowFormula>Table2[[#Totals],[Absolute difference '[kWh']]]/Table2[[#Totals],[Increment DSO '[kWh']]]</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -569,13 +2821,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{040A8FA8-D6C5-B341-BBC7-C08B544AAD74}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="11" bestFit="1" customWidth="1"/>
@@ -584,11 +2836,12 @@
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="26.1640625" customWidth="1"/>
+    <col min="11" max="11" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -614,13 +2867,19 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" s="1">
         <v>45884.568055555559</v>
       </c>
@@ -641,9 +2900,22 @@
         <f>6.741-8.6</f>
         <v>-1.859</v>
       </c>
-      <c r="J2" s="3"/>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2" s="4">
+        <f>Table2[[#This Row],[Total EnergyMe '[kWh']]]-Table2[[#This Row],[Total DSO '[kWh']]]</f>
+        <v>0</v>
+      </c>
+      <c r="L2" s="3" t="e">
+        <f>Table2[[#This Row],[Absolute difference '[kWh']]]/Table2[[#This Row],[Total DSO '[kWh']]]</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12">
       <c r="A3" s="1">
         <v>45884.867361111108</v>
       </c>
@@ -667,20 +2939,28 @@
         <f>E3-E2</f>
         <v>3</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="4">
         <f t="shared" ref="H3" si="0">F3-F2</f>
         <v>2.9430000000000001</v>
       </c>
-      <c r="I3" s="5">
-        <f>Table2[[#This Row],[Increment EnergyMe '[kWh']]]-Table2[[#This Row],[Increment DSO '[kWh']]]</f>
+      <c r="I3" s="4">
+        <f>G3+I2</f>
+        <v>3</v>
+      </c>
+      <c r="J3" s="4">
+        <f>H3+J2</f>
+        <v>2.9430000000000001</v>
+      </c>
+      <c r="K3" s="4">
+        <f>Table2[[#This Row],[Total EnergyMe '[kWh']]]-Table2[[#This Row],[Total DSO '[kWh']]]</f>
         <v>-5.699999999999994E-2</v>
       </c>
-      <c r="J3" s="3">
-        <f>Table2[[#This Row],[Absolute difference '[kWh']]]/Table2[[#This Row],[Increment DSO '[kWh']]]</f>
+      <c r="L3" s="3">
+        <f>Table2[[#This Row],[Absolute difference '[kWh']]]/Table2[[#This Row],[Total DSO '[kWh']]]</f>
         <v>-1.8999999999999979E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12">
       <c r="A4" s="1">
         <v>45885.563888888886</v>
       </c>
@@ -704,20 +2984,28 @@
         <f>E4-E3</f>
         <v>7</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="4">
         <f t="shared" ref="H4" si="1">F4-F3</f>
         <v>6.1059999999999999</v>
       </c>
-      <c r="I4" s="5">
-        <f>Table2[[#This Row],[Increment EnergyMe '[kWh']]]-Table2[[#This Row],[Increment DSO '[kWh']]]</f>
-        <v>-0.89400000000000013</v>
-      </c>
-      <c r="J4" s="3">
-        <f>Table2[[#This Row],[Absolute difference '[kWh']]]/Table2[[#This Row],[Increment DSO '[kWh']]]</f>
-        <v>-0.12771428571428572</v>
+      <c r="I4" s="4">
+        <f t="shared" ref="I4:I7" si="2">G4+I3</f>
+        <v>10</v>
+      </c>
+      <c r="J4" s="4">
+        <f t="shared" ref="J4:J7" si="3">H4+J3</f>
+        <v>9.0489999999999995</v>
+      </c>
+      <c r="K4" s="4">
+        <f>Table2[[#This Row],[Total EnergyMe '[kWh']]]-Table2[[#This Row],[Total DSO '[kWh']]]</f>
+        <v>-0.95100000000000051</v>
+      </c>
+      <c r="L4" s="3">
+        <f>Table2[[#This Row],[Absolute difference '[kWh']]]/Table2[[#This Row],[Total DSO '[kWh']]]</f>
+        <v>-9.5100000000000046E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
       <c r="A5" s="1">
         <v>45885.840277777781</v>
       </c>
@@ -741,20 +3029,28 @@
         <f>E5-E4</f>
         <v>1</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="4">
         <f>F5-F4</f>
         <v>2.5330000000000004</v>
       </c>
-      <c r="I5" s="5">
-        <f>Table2[[#This Row],[Increment EnergyMe '[kWh']]]-Table2[[#This Row],[Increment DSO '[kWh']]]</f>
-        <v>1.5330000000000004</v>
-      </c>
-      <c r="J5" s="3">
-        <f>Table2[[#This Row],[Absolute difference '[kWh']]]/Table2[[#This Row],[Increment DSO '[kWh']]]</f>
-        <v>1.5330000000000004</v>
+      <c r="I5" s="4">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="J5" s="4">
+        <f t="shared" si="3"/>
+        <v>11.582000000000001</v>
+      </c>
+      <c r="K5" s="4">
+        <f>Table2[[#This Row],[Total EnergyMe '[kWh']]]-Table2[[#This Row],[Total DSO '[kWh']]]</f>
+        <v>0.58200000000000074</v>
+      </c>
+      <c r="L5" s="3">
+        <f>Table2[[#This Row],[Absolute difference '[kWh']]]/Table2[[#This Row],[Total DSO '[kWh']]]</f>
+        <v>5.2909090909090975E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12">
       <c r="A6" s="1">
         <v>45886.49722222222</v>
       </c>
@@ -778,45 +3074,127 @@
         <f>E6-E5</f>
         <v>7</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="4">
         <f>F6-F5</f>
         <v>5.8887</v>
       </c>
-      <c r="I6" s="5">
-        <f>Table2[[#This Row],[Increment EnergyMe '[kWh']]]-Table2[[#This Row],[Increment DSO '[kWh']]]</f>
-        <v>-1.1113</v>
-      </c>
-      <c r="J6" s="3">
-        <f>Table2[[#This Row],[Absolute difference '[kWh']]]/Table2[[#This Row],[Increment DSO '[kWh']]]</f>
-        <v>-0.15875714285714285</v>
+      <c r="I6" s="4">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="J6" s="4">
+        <f t="shared" si="3"/>
+        <v>17.470700000000001</v>
+      </c>
+      <c r="K6" s="4">
+        <f>Table2[[#This Row],[Total EnergyMe '[kWh']]]-Table2[[#This Row],[Total DSO '[kWh']]]</f>
+        <v>-0.52929999999999922</v>
+      </c>
+      <c r="L6" s="3">
+        <f>Table2[[#This Row],[Absolute difference '[kWh']]]/Table2[[#This Row],[Total DSO '[kWh']]]</f>
+        <v>-2.9405555555555511E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>10</v>
+    <row r="7" spans="1:12">
+      <c r="A7" s="1">
+        <v>45886.902777777781</v>
+      </c>
+      <c r="B7">
+        <v>1602</v>
+      </c>
+      <c r="C7">
+        <v>1356</v>
+      </c>
+      <c r="D7">
+        <v>2168</v>
+      </c>
+      <c r="E7">
+        <f>SUM(Table2[[#This Row],[F1 '[kWh']]:[F3  '[kWh']]])</f>
+        <v>5126</v>
+      </c>
+      <c r="F7" s="2">
+        <v>20.601299999999998</v>
       </c>
       <c r="G7">
-        <f>SUBTOTAL(109,Table2[Increment DSO '[kWh']])</f>
-        <v>18</v>
-      </c>
-      <c r="H7" s="5">
-        <f>SUBTOTAL(109,Table2[Increment EnergyMe '[kWh']])</f>
-        <v>17.470700000000001</v>
-      </c>
-      <c r="I7">
-        <f>Table2[[#Totals],[Increment EnergyMe '[kWh']]]-Table2[[#Totals],[Increment DSO '[kWh']]]</f>
-        <v>-0.52929999999999922</v>
+        <f>E7-E6</f>
+        <v>5</v>
+      </c>
+      <c r="H7" s="4">
+        <f>F7-F6</f>
+        <v>4.9895999999999976</v>
+      </c>
+      <c r="I7" s="4">
+        <f t="shared" si="2"/>
+        <v>23</v>
       </c>
       <c r="J7" s="4">
-        <f>Table2[[#Totals],[Absolute difference '[kWh']]]/Table2[[#Totals],[Increment DSO '[kWh']]]</f>
-        <v>-2.9405555555555511E-2</v>
-      </c>
+        <f t="shared" si="3"/>
+        <v>22.460299999999997</v>
+      </c>
+      <c r="K7" s="4">
+        <f>Table2[[#This Row],[Total EnergyMe '[kWh']]]-Table2[[#This Row],[Total DSO '[kWh']]]</f>
+        <v>-0.5397000000000034</v>
+      </c>
+      <c r="L7" s="3">
+        <f>Table2[[#This Row],[Absolute difference '[kWh']]]/Table2[[#This Row],[Total DSO '[kWh']]]</f>
+        <v>-2.3465217391304496E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="1">
+        <v>45887.631944444445</v>
+      </c>
+      <c r="B8">
+        <v>1605</v>
+      </c>
+      <c r="C8">
+        <v>1356</v>
+      </c>
+      <c r="D8">
+        <v>2172</v>
+      </c>
+      <c r="E8">
+        <f>SUM(Table2[[#This Row],[F1 '[kWh']]:[F3  '[kWh']]])</f>
+        <v>5133</v>
+      </c>
+      <c r="F8" s="2">
+        <v>28.2</v>
+      </c>
+      <c r="G8">
+        <f>E8-E7</f>
+        <v>7</v>
+      </c>
+      <c r="H8" s="4">
+        <f>F8-F7</f>
+        <v>7.5987000000000009</v>
+      </c>
+      <c r="I8" s="4">
+        <f t="shared" ref="I8" si="4">G8+I7</f>
+        <v>30</v>
+      </c>
+      <c r="J8" s="4">
+        <f t="shared" ref="J8" si="5">H8+J7</f>
+        <v>30.058999999999997</v>
+      </c>
+      <c r="K8" s="4">
+        <f>Table2[[#This Row],[Total EnergyMe '[kWh']]]-Table2[[#This Row],[Total DSO '[kWh']]]</f>
+        <v>5.8999999999997499E-2</v>
+      </c>
+      <c r="L8" s="3">
+        <f>Table2[[#This Row],[Absolute difference '[kWh']]]/Table2[[#This Row],[Total DSO '[kWh']]]</f>
+        <v>1.9666666666665832E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="7:7">
+      <c r="G38" s="5"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
On the way to make HTTPS OTA work
</commit_message>
<xml_diff>
--- a/source/DSO comparison.xlsx
+++ b/source/DSO comparison.xlsx
@@ -1,37 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jibrilsharafi/Personal/EnergyMe-Home/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C8E707-47AC-5142-BA9F-E04255100E66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F68804-8EEB-7C43-8EEA-47EA22917872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{F09C8B9D-A9D0-9640-90EA-F6C802E5DACE}"/>
   </bookViews>
   <sheets>
     <sheet name="Scalea" sheetId="2" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Scalea!$A$2:$A$8</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Scalea!$K$1</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Scalea!$A$2:$A$8</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Scalea!$K$1</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Scalea!$K$2:$K$8</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Scalea!$L$1</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Scalea!$L$2:$L$8</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Scalea!$K$2:$K$8</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Scalea!$L$1</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Scalea!$L$2:$L$8</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Scalea!$A$2:$A$8</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Scalea!$K$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Scalea!$K$2:$K$8</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Scalea!$L$1</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Scalea!$L$2:$L$8</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -336,7 +319,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-IT"/>
+          <a:endParaRPr lang="en-GB"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -386,10 +369,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Scalea!$A$2:$A$8</c:f>
+              <c:f>Scalea!$A$2:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy\ h:mm</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>45884.568055555559</c:v>
                 </c:pt>
@@ -410,16 +393,31 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>45887.631944444445</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45888.495833333334</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45890.913888888892</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45891.475694444445</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45893.56527777778</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>45895.414583333331</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Scalea!$I$2:$I$8</c:f>
+              <c:f>Scalea!$I$2:$I$13</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>0</c:v>
                 </c:pt>
@@ -440,6 +438,21 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>142</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>209</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -491,10 +504,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Scalea!$A$2:$A$8</c:f>
+              <c:f>Scalea!$A$2:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy\ h:mm</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>45884.568055555559</c:v>
                 </c:pt>
@@ -515,16 +528,31 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>45887.631944444445</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45888.495833333334</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45890.913888888892</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45891.475694444445</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45893.56527777778</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>45895.414583333331</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Scalea!$J$2:$J$8</c:f>
+              <c:f>Scalea!$J$2:$J$13</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>0</c:v>
                 </c:pt>
@@ -545,6 +573,21 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>30.058999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>37.853300000000004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>65.018000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>73.093800000000016</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>141.31200000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>206.2345</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -844,7 +887,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-IT"/>
+          <a:endParaRPr lang="en-GB"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -894,10 +937,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Scalea!$A$2:$A$8</c:f>
+              <c:f>Scalea!$A$2:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy\ h:mm</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>45884.568055555559</c:v>
                 </c:pt>
@@ -918,16 +961,31 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>45887.631944444445</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45888.495833333334</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45890.913888888892</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45891.475694444445</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45893.56527777778</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>45895.414583333331</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Scalea!$K$2:$K$8</c:f>
+              <c:f>Scalea!$K$2:$K$13</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -948,6 +1006,21 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>5.8999999999997499E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-1.1466999999999956</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-1.9819999999999993</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-1.9061999999999841</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.68799999999998818</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-2.765500000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -999,10 +1072,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Scalea!$A$2:$A$8</c:f>
+              <c:f>Scalea!$A$2:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy\ h:mm</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>45884.568055555559</c:v>
                 </c:pt>
@@ -1023,16 +1096,31 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>45887.631944444445</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45888.495833333334</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45890.913888888892</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45891.475694444445</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45893.56527777778</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>45895.414583333331</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Scalea!$L$2:$L$8</c:f>
+              <c:f>Scalea!$L$2:$L$13</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1053,6 +1141,21 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1.9666666666665832E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-2.9402564102563991E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-2.9582089552238795E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-2.5415999999999789E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-4.8450704225351283E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-1.3232057416267956E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2399,15 +2502,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>297180</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>5080</xdr:rowOff>
+      <xdr:colOff>119380</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1536700</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2434,16 +2537,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>1366520</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1671320</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>172720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2474,8 +2577,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4C15CE87-9103-3543-9609-61C6C7FA6FB0}" name="Table2" displayName="Table2" ref="A1:L8">
-  <autoFilter ref="A1:L8" xr:uid="{4C15CE87-9103-3543-9609-61C6C7FA6FB0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4C15CE87-9103-3543-9609-61C6C7FA6FB0}" name="Table2" displayName="Table2" ref="A1:L13">
+  <autoFilter ref="A1:L13" xr:uid="{4C15CE87-9103-3543-9609-61C6C7FA6FB0}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{A85D948A-57A5-5F43-A54C-ACFC33A5E4FB}" name="Timestamp" totalsRowLabel="Total" dataDxfId="11"/>
     <tableColumn id="2" xr3:uid="{D6F6B36F-5FCE-A84C-978A-9C1F96ED9634}" name="F1 [kWh]"/>
@@ -2821,22 +2924,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{040A8FA8-D6C5-B341-BBC7-C08B544AAD74}">
-  <dimension ref="A1:L38"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="26.1640625" customWidth="1"/>
+    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="25.5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="24.83203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -2936,11 +3040,11 @@
         <v>1.0840000000000001</v>
       </c>
       <c r="G3">
-        <f>E3-E2</f>
+        <f t="shared" ref="G3:G8" si="0">E3-E2</f>
         <v>3</v>
       </c>
       <c r="H3" s="4">
-        <f t="shared" ref="H3" si="0">F3-F2</f>
+        <f t="shared" ref="H3" si="1">F3-F2</f>
         <v>2.9430000000000001</v>
       </c>
       <c r="I3" s="4">
@@ -2981,19 +3085,19 @@
         <v>7.19</v>
       </c>
       <c r="G4">
-        <f>E4-E3</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="H4" s="4">
-        <f t="shared" ref="H4" si="1">F4-F3</f>
+        <f t="shared" ref="H4" si="2">F4-F3</f>
         <v>6.1059999999999999</v>
       </c>
       <c r="I4" s="4">
-        <f t="shared" ref="I4:I7" si="2">G4+I3</f>
+        <f t="shared" ref="I4:I7" si="3">G4+I3</f>
         <v>10</v>
       </c>
       <c r="J4" s="4">
-        <f t="shared" ref="J4:J7" si="3">H4+J3</f>
+        <f t="shared" ref="J4:J7" si="4">H4+J3</f>
         <v>9.0489999999999995</v>
       </c>
       <c r="K4" s="4">
@@ -3026,19 +3130,19 @@
         <v>9.7230000000000008</v>
       </c>
       <c r="G5">
-        <f>E5-E4</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H5" s="4">
-        <f>F5-F4</f>
+        <f t="shared" ref="H5:H11" si="5">F5-F4</f>
         <v>2.5330000000000004</v>
       </c>
       <c r="I5" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="J5" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>11.582000000000001</v>
       </c>
       <c r="K5" s="4">
@@ -3071,19 +3175,19 @@
         <v>15.611700000000001</v>
       </c>
       <c r="G6">
-        <f>E6-E5</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="H6" s="4">
-        <f>F6-F5</f>
+        <f t="shared" si="5"/>
         <v>5.8887</v>
       </c>
       <c r="I6" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="J6" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>17.470700000000001</v>
       </c>
       <c r="K6" s="4">
@@ -3116,19 +3220,19 @@
         <v>20.601299999999998</v>
       </c>
       <c r="G7">
-        <f>E7-E6</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="H7" s="4">
-        <f>F7-F6</f>
+        <f t="shared" si="5"/>
         <v>4.9895999999999976</v>
       </c>
       <c r="I7" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="J7" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>22.460299999999997</v>
       </c>
       <c r="K7" s="4">
@@ -3161,19 +3265,19 @@
         <v>28.2</v>
       </c>
       <c r="G8">
-        <f>E8-E7</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="H8" s="4">
-        <f>F8-F7</f>
+        <f t="shared" si="5"/>
         <v>7.5987000000000009</v>
       </c>
       <c r="I8" s="4">
-        <f t="shared" ref="I8" si="4">G8+I7</f>
+        <f t="shared" ref="I8" si="6">G8+I7</f>
         <v>30</v>
       </c>
       <c r="J8" s="4">
-        <f t="shared" ref="J8" si="5">H8+J7</f>
+        <f t="shared" ref="J8" si="7">H8+J7</f>
         <v>30.058999999999997</v>
       </c>
       <c r="K8" s="4">
@@ -3185,8 +3289,243 @@
         <v>1.9666666666665832E-3</v>
       </c>
     </row>
-    <row r="38" spans="7:7">
+    <row r="9" spans="1:12">
+      <c r="A9" s="1">
+        <v>45888.495833333334</v>
+      </c>
+      <c r="B9">
+        <v>1608</v>
+      </c>
+      <c r="C9">
+        <v>1359</v>
+      </c>
+      <c r="D9">
+        <v>2175</v>
+      </c>
+      <c r="E9">
+        <f>SUM(Table2[[#This Row],[F1 '[kWh']]:[F3  '[kWh']]])</f>
+        <v>5142</v>
+      </c>
+      <c r="F9" s="2">
+        <v>35.994300000000003</v>
+      </c>
+      <c r="G9">
+        <f t="shared" ref="G9" si="8">E9-E8</f>
+        <v>9</v>
+      </c>
+      <c r="H9" s="4">
+        <f t="shared" si="5"/>
+        <v>7.7943000000000033</v>
+      </c>
+      <c r="I9" s="4">
+        <f t="shared" ref="I9" si="9">G9+I8</f>
+        <v>39</v>
+      </c>
+      <c r="J9" s="4">
+        <f t="shared" ref="J9" si="10">H9+J8</f>
+        <v>37.853300000000004</v>
+      </c>
+      <c r="K9" s="4">
+        <f>Table2[[#This Row],[Total EnergyMe '[kWh']]]-Table2[[#This Row],[Total DSO '[kWh']]]</f>
+        <v>-1.1466999999999956</v>
+      </c>
+      <c r="L9" s="3">
+        <f>Table2[[#This Row],[Absolute difference '[kWh']]]/Table2[[#This Row],[Total DSO '[kWh']]]</f>
+        <v>-2.9402564102563991E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="1">
+        <v>45890.913888888892</v>
+      </c>
+      <c r="B10">
+        <v>1621</v>
+      </c>
+      <c r="C10">
+        <v>1367</v>
+      </c>
+      <c r="D10">
+        <v>2182</v>
+      </c>
+      <c r="E10">
+        <f>SUM(Table2[[#This Row],[F1 '[kWh']]:[F3  '[kWh']]])</f>
+        <v>5170</v>
+      </c>
+      <c r="F10" s="2">
+        <v>63.158999999999999</v>
+      </c>
+      <c r="G10">
+        <f t="shared" ref="G10" si="11">E10-E9</f>
+        <v>28</v>
+      </c>
+      <c r="H10" s="4">
+        <f t="shared" si="5"/>
+        <v>27.164699999999996</v>
+      </c>
+      <c r="I10" s="4">
+        <f t="shared" ref="I10" si="12">G10+I9</f>
+        <v>67</v>
+      </c>
+      <c r="J10" s="4">
+        <f t="shared" ref="J10" si="13">H10+J9</f>
+        <v>65.018000000000001</v>
+      </c>
+      <c r="K10" s="4">
+        <f>Table2[[#This Row],[Total EnergyMe '[kWh']]]-Table2[[#This Row],[Total DSO '[kWh']]]</f>
+        <v>-1.9819999999999993</v>
+      </c>
+      <c r="L10" s="3">
+        <f>Table2[[#This Row],[Absolute difference '[kWh']]]/Table2[[#This Row],[Total DSO '[kWh']]]</f>
+        <v>-2.9582089552238795E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="1">
+        <v>45891.475694444445</v>
+      </c>
+      <c r="B11">
+        <v>1623</v>
+      </c>
+      <c r="C11">
+        <v>1368</v>
+      </c>
+      <c r="D11">
+        <v>2187</v>
+      </c>
+      <c r="E11">
+        <f>SUM(Table2[[#This Row],[F1 '[kWh']]:[F3  '[kWh']]])</f>
+        <v>5178</v>
+      </c>
+      <c r="F11" s="2">
+        <v>71.234800000000007</v>
+      </c>
+      <c r="G11">
+        <f t="shared" ref="G11" si="14">E11-E10</f>
+        <v>8</v>
+      </c>
+      <c r="H11" s="4">
+        <f t="shared" si="5"/>
+        <v>8.0758000000000081</v>
+      </c>
+      <c r="I11" s="4">
+        <f t="shared" ref="I11" si="15">G11+I10</f>
+        <v>75</v>
+      </c>
+      <c r="J11" s="4">
+        <f t="shared" ref="J11" si="16">H11+J10</f>
+        <v>73.093800000000016</v>
+      </c>
+      <c r="K11" s="4">
+        <f>Table2[[#This Row],[Total EnergyMe '[kWh']]]-Table2[[#This Row],[Total DSO '[kWh']]]</f>
+        <v>-1.9061999999999841</v>
+      </c>
+      <c r="L11" s="3">
+        <f>Table2[[#This Row],[Absolute difference '[kWh']]]/Table2[[#This Row],[Total DSO '[kWh']]]</f>
+        <v>-2.5415999999999789E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="1">
+        <v>45893.56527777778</v>
+      </c>
+      <c r="B12">
+        <v>1625</v>
+      </c>
+      <c r="C12">
+        <v>1392</v>
+      </c>
+      <c r="D12">
+        <v>2228</v>
+      </c>
+      <c r="E12">
+        <f>SUM(Table2[[#This Row],[F1 '[kWh']]:[F3  '[kWh']]])</f>
+        <v>5245</v>
+      </c>
+      <c r="F12" s="2">
+        <v>139.453</v>
+      </c>
+      <c r="G12">
+        <f t="shared" ref="G12" si="17">E12-E11</f>
+        <v>67</v>
+      </c>
+      <c r="H12" s="4">
+        <f t="shared" ref="H12" si="18">F12-F11</f>
+        <v>68.218199999999996</v>
+      </c>
+      <c r="I12" s="4">
+        <f t="shared" ref="I12" si="19">G12+I11</f>
+        <v>142</v>
+      </c>
+      <c r="J12" s="4">
+        <f t="shared" ref="J12" si="20">H12+J11</f>
+        <v>141.31200000000001</v>
+      </c>
+      <c r="K12" s="4">
+        <f>Table2[[#This Row],[Total EnergyMe '[kWh']]]-Table2[[#This Row],[Total DSO '[kWh']]]</f>
+        <v>-0.68799999999998818</v>
+      </c>
+      <c r="L12" s="3">
+        <f>Table2[[#This Row],[Absolute difference '[kWh']]]/Table2[[#This Row],[Total DSO '[kWh']]]</f>
+        <v>-4.8450704225351283E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="1">
+        <v>45895.414583333331</v>
+      </c>
+      <c r="B13">
+        <v>1632</v>
+      </c>
+      <c r="C13">
+        <v>1405</v>
+      </c>
+      <c r="D13">
+        <v>2275</v>
+      </c>
+      <c r="E13">
+        <f>SUM(Table2[[#This Row],[F1 '[kWh']]:[F3  '[kWh']]])</f>
+        <v>5312</v>
+      </c>
+      <c r="F13" s="2">
+        <v>204.37549999999999</v>
+      </c>
+      <c r="G13">
+        <f t="shared" ref="G13" si="21">E13-E12</f>
+        <v>67</v>
+      </c>
+      <c r="H13" s="4">
+        <f t="shared" ref="H13" si="22">F13-F12</f>
+        <v>64.922499999999985</v>
+      </c>
+      <c r="I13" s="4">
+        <f t="shared" ref="I13" si="23">G13+I12</f>
+        <v>209</v>
+      </c>
+      <c r="J13" s="4">
+        <f t="shared" ref="J13" si="24">H13+J12</f>
+        <v>206.2345</v>
+      </c>
+      <c r="K13" s="4">
+        <f>Table2[[#This Row],[Total EnergyMe '[kWh']]]-Table2[[#This Row],[Total DSO '[kWh']]]</f>
+        <v>-2.765500000000003</v>
+      </c>
+      <c r="L13" s="3">
+        <f>Table2[[#This Row],[Absolute difference '[kWh']]]/Table2[[#This Row],[Total DSO '[kWh']]]</f>
+        <v>-1.3232057416267956E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="5:7">
+      <c r="E37" s="5"/>
+    </row>
+    <row r="38" spans="5:7">
+      <c r="E38" s="5"/>
       <c r="G38" s="5"/>
+    </row>
+    <row r="40" spans="5:7">
+      <c r="E40" s="5"/>
+    </row>
+    <row r="41" spans="5:7">
+      <c r="E41" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>